<commit_message>
Sketches and screenshots added
</commit_message>
<xml_diff>
--- a/qual/data/AFG_asylum-decisions_2021.xlsx
+++ b/qual/data/AFG_asylum-decisions_2021.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tatianakalainoff/Documents/GitHub/major-studio/qual/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E94CBB43-90D5-FE4D-86AA-6E57FFE5882A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765DC1B5-7D92-F740-BB6E-8224F39F0025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15640" xr2:uid="{8891801E-EAFB-D045-83BA-51454144F761}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16080" xr2:uid="{8891801E-EAFB-D045-83BA-51454144F761}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$97</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -863,11 +866,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4EF9F0-6A9F-EB41-88D2-2B7809C1518A}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M97"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M105" sqref="M105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="25.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4847,6 +4853,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M97" xr:uid="{3F4EF9F0-6A9F-EB41-88D2-2B7809C1518A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>